<commit_message>
Updated GHI data. Added '4.5' as float value for the string '<5' present in the pristine dataset
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/IFPRI-GHI/IFPRI-GHI.xlsx
+++ b/Simple_XLS_Importer/data/IFPRI-GHI/IFPRI-GHI.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="525" windowWidth="17415" windowHeight="5835" activeTab="1"/>
+    <workbookView xWindow="750" yWindow="525" windowWidth="17415" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
     <sheet name="metadata" sheetId="4" r:id="rId2"/>
+    <sheet name="NOTES" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="129">
   <si>
     <t>indicator_internal_id</t>
   </si>
@@ -399,6 +400,9 @@
   </si>
   <si>
     <t>GHI</t>
+  </si>
+  <si>
+    <t>For the countries that the value was "&lt;5" (or "&lt;55" corner cases), there was set up a 4.5 value</t>
   </si>
 </sst>
 </file>
@@ -427,12 +431,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -462,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,6 +488,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C498" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C513" sqref="C513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1081,7 +1094,9 @@
       <c r="B27" s="3">
         <v>2015</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="12.75">
       <c r="A28" s="3" t="s">
@@ -1277,7 +1292,9 @@
       <c r="B45" s="3">
         <v>2015</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="12.75">
       <c r="A46" s="3" t="s">
@@ -1286,7 +1303,9 @@
       <c r="B46" s="3">
         <v>1995</v>
       </c>
-      <c r="C46" s="5"/>
+      <c r="C46" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="12.75">
       <c r="A47" s="3" t="s">
@@ -1295,7 +1314,9 @@
       <c r="B47" s="3">
         <v>2000</v>
       </c>
-      <c r="C47" s="5"/>
+      <c r="C47" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="12.75">
       <c r="A48" s="3" t="s">
@@ -1304,7 +1325,9 @@
       <c r="B48" s="3">
         <v>2005</v>
       </c>
-      <c r="C48" s="5"/>
+      <c r="C48" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="12.75">
       <c r="A49" s="3" t="s">
@@ -1423,7 +1446,9 @@
       <c r="B59" s="3">
         <v>2015</v>
       </c>
-      <c r="C59" s="5"/>
+      <c r="C59" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="12.75">
       <c r="A60" s="3" t="s">
@@ -1520,7 +1545,9 @@
       <c r="B68" s="3">
         <v>2015</v>
       </c>
-      <c r="C68" s="5"/>
+      <c r="C68" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="69" spans="1:3" ht="12.75">
       <c r="A69" s="3" t="s">
@@ -1903,7 +1930,9 @@
       <c r="B103" s="3">
         <v>2015</v>
       </c>
-      <c r="C103" s="5"/>
+      <c r="C103" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="104" spans="1:3" ht="12.75">
       <c r="A104" s="3" t="s">
@@ -1923,7 +1952,9 @@
       <c r="B105" s="3">
         <v>1995</v>
       </c>
-      <c r="C105" s="5"/>
+      <c r="C105" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="106" spans="1:3" ht="12.75">
       <c r="A106" s="3" t="s">
@@ -1932,7 +1963,9 @@
       <c r="B106" s="3">
         <v>2000</v>
       </c>
-      <c r="C106" s="5"/>
+      <c r="C106" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="107" spans="1:3" ht="12.75">
       <c r="A107" s="3" t="s">
@@ -1941,7 +1974,9 @@
       <c r="B107" s="3">
         <v>2005</v>
       </c>
-      <c r="C107" s="5"/>
+      <c r="C107" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="108" spans="1:3" ht="12.75">
       <c r="A108" s="3" t="s">
@@ -2115,7 +2150,9 @@
       <c r="B123" s="3">
         <v>2015</v>
       </c>
-      <c r="C123" s="5"/>
+      <c r="C123" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="124" spans="1:3" ht="12.75">
       <c r="A124" s="3" t="s">
@@ -2212,7 +2249,9 @@
       <c r="B132" s="3">
         <v>2015</v>
       </c>
-      <c r="C132" s="5"/>
+      <c r="C132" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="133" spans="1:3" ht="12.75">
       <c r="A133" s="3" t="s">
@@ -2243,7 +2282,9 @@
       <c r="B135" s="3">
         <v>2005</v>
       </c>
-      <c r="C135" s="5"/>
+      <c r="C135" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="136" spans="1:3" ht="12.75">
       <c r="A136" s="3" t="s">
@@ -2252,7 +2293,9 @@
       <c r="B136" s="3">
         <v>2015</v>
       </c>
-      <c r="C136" s="5"/>
+      <c r="C136" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="137" spans="1:3" ht="12.75">
       <c r="A137" s="3" t="s">
@@ -2283,7 +2326,9 @@
       <c r="B139" s="3">
         <v>2005</v>
       </c>
-      <c r="C139" s="5"/>
+      <c r="C139" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="140" spans="1:3" ht="12.75">
       <c r="A140" s="3" t="s">
@@ -2622,7 +2667,9 @@
       <c r="B170" s="3">
         <v>2015</v>
       </c>
-      <c r="C170" s="5"/>
+      <c r="C170" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="171" spans="1:3" ht="12.75">
       <c r="A171" s="3" t="s">
@@ -3764,7 +3811,9 @@
       <c r="B274" s="3">
         <v>2000</v>
       </c>
-      <c r="C274" s="5"/>
+      <c r="C274" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="275" spans="1:3" ht="12.75">
       <c r="A275" s="3" t="s">
@@ -3773,7 +3822,9 @@
       <c r="B275" s="3">
         <v>2005</v>
       </c>
-      <c r="C275" s="5"/>
+      <c r="C275" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="276" spans="1:3" ht="12.75">
       <c r="A276" s="3" t="s">
@@ -3881,7 +3932,9 @@
       <c r="B285" s="3">
         <v>2015</v>
       </c>
-      <c r="C285" s="5"/>
+      <c r="C285" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="286" spans="1:3" ht="12.75">
       <c r="A286" s="3" t="s">
@@ -4066,7 +4119,9 @@
       <c r="B302" s="3">
         <v>2015</v>
       </c>
-      <c r="C302" s="5"/>
+      <c r="C302" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="303" spans="1:3" ht="12.75">
       <c r="A303" s="3" t="s">
@@ -4548,7 +4603,9 @@
       <c r="B346" s="3">
         <v>2015</v>
       </c>
-      <c r="C346" s="5"/>
+      <c r="C346" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="347" spans="1:3" ht="12.75">
       <c r="A347" s="3" t="s">
@@ -6350,7 +6407,9 @@
       <c r="B510" s="3">
         <v>2015</v>
       </c>
-      <c r="C510" s="5"/>
+      <c r="C510" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="511" spans="1:3" ht="12.75">
       <c r="A511" s="3" t="s">
@@ -6381,7 +6440,9 @@
       <c r="B513" s="3">
         <v>2005</v>
       </c>
-      <c r="C513" s="5"/>
+      <c r="C513" s="7">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="514" spans="1:3" ht="12.75">
       <c r="A514" s="3" t="s">
@@ -8045,7 +8106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -8090,4 +8151,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>